<commit_message>
Initial additions and examples
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-PADI-AutopsyObservation.xlsx
+++ b/output/StructureDefinition-PADI-AutopsyObservation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="411">
   <si>
     <t>Path</t>
   </si>
@@ -469,6 +469,9 @@
     <t>Need to track the status of individual results. Some results are finalized before the whole report is finalized.</t>
   </si>
   <si>
+    <t>final</t>
+  </si>
+  <si>
     <t>required</t>
   </si>
   <si>
@@ -541,6 +544,14 @@
   </si>
   <si>
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
+  </si>
+  <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://loinc.org"/&gt;
+    &lt;code value="75782-3"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
     <t>example</t>
@@ -3027,7 +3038,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
         <v>139</v>
       </c>
@@ -3043,7 +3054,7 @@
         <v>55</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>56</v>
@@ -3074,7 +3085,7 @@
         <v>45</v>
       </c>
       <c r="R14" t="s" s="2">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="S14" t="s" s="2">
         <v>45</v>
@@ -3089,13 +3100,13 @@
         <v>45</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>45</v>
@@ -3128,19 +3139,19 @@
         <v>67</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AO14" t="s" s="2">
         <v>45</v>
@@ -3148,7 +3159,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3171,19 +3182,19 @@
         <v>45</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="O15" t="s" s="2">
         <v>45</v>
@@ -3211,10 +3222,10 @@
         <v>79</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3232,7 +3243,7 @@
         <v>45</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>43</v>
@@ -3256,10 +3267,10 @@
         <v>45</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3267,11 +3278,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3290,19 +3301,19 @@
         <v>56</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3312,7 +3323,7 @@
         <v>45</v>
       </c>
       <c r="R16" t="s" s="2">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="S16" t="s" s="2">
         <v>45</v>
@@ -3327,13 +3338,13 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3351,7 +3362,7 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>55</v>
@@ -3366,27 +3377,27 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3409,19 +3420,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3470,7 +3481,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3485,19 +3496,19 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3505,7 +3516,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3528,16 +3539,16 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3587,7 +3598,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3608,13 +3619,13 @@
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3622,11 +3633,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3645,19 +3656,19 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
@@ -3706,7 +3717,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3721,19 +3732,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3741,11 +3752,11 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3764,19 +3775,19 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3825,7 +3836,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3840,19 +3851,19 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3860,7 +3871,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3883,16 +3894,16 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3942,7 +3953,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3963,13 +3974,13 @@
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -3977,7 +3988,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4000,17 +4011,17 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4059,7 +4070,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4074,27 +4085,27 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4102,13 +4113,13 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>55</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>45</v>
@@ -4117,19 +4128,19 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4178,7 +4189,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4187,7 +4198,7 @@
         <v>55</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>67</v>
@@ -4196,24 +4207,24 @@
         <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4236,19 +4247,19 @@
         <v>45</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4273,13 +4284,13 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4297,7 +4308,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4306,7 +4317,7 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
@@ -4321,7 +4332,7 @@
         <v>98</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
@@ -4332,11 +4343,11 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4355,19 +4366,19 @@
         <v>45</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4392,13 +4403,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4416,7 +4427,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4434,24 +4445,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4474,19 +4485,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4535,7 +4546,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4556,10 +4567,10 @@
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -4570,7 +4581,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4593,16 +4604,16 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4628,13 +4639,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4652,7 +4663,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4670,24 +4681,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4710,19 +4721,19 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4747,13 +4758,13 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
@@ -4771,7 +4782,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4792,10 +4803,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4806,7 +4817,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4829,16 +4840,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4888,7 +4899,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4906,24 +4917,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4946,16 +4957,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5005,7 +5016,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5023,24 +5034,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5063,19 +5074,19 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5124,7 +5135,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5136,7 +5147,7 @@
         <v>45</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>45</v>
@@ -5145,10 +5156,10 @@
         <v>45</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5159,7 +5170,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5185,10 +5196,10 @@
         <v>57</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5239,7 +5250,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5263,7 +5274,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5274,7 +5285,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5303,7 +5314,7 @@
         <v>102</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>104</v>
@@ -5356,7 +5367,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5380,7 +5391,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5391,11 +5402,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5417,10 +5428,10 @@
         <v>101</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>104</v>
@@ -5475,7 +5486,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5510,7 +5521,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5533,13 +5544,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5590,7 +5601,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5599,7 +5610,7 @@
         <v>55</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>67</v>
@@ -5611,10 +5622,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5625,7 +5636,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5648,13 +5659,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5705,7 +5716,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5714,7 +5725,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5726,10 +5737,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5740,7 +5751,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5763,19 +5774,19 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5803,10 +5814,10 @@
         <v>79</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
@@ -5824,7 +5835,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5842,13 +5853,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5859,7 +5870,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5882,19 +5893,19 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5919,13 +5930,13 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
@@ -5943,7 +5954,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5961,13 +5972,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5978,7 +5989,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6001,17 +6012,17 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6060,7 +6071,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6084,7 +6095,7 @@
         <v>45</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6095,7 +6106,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6121,10 +6132,10 @@
         <v>57</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -6175,7 +6186,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6196,10 +6207,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6210,7 +6221,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6233,16 +6244,16 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -6292,7 +6303,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6313,10 +6324,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6327,7 +6338,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6350,16 +6361,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6409,7 +6420,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6430,10 +6441,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6444,7 +6455,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6467,19 +6478,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -6528,7 +6539,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6549,10 +6560,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6563,7 +6574,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6589,10 +6600,10 @@
         <v>57</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6643,7 +6654,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6667,7 +6678,7 @@
         <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6678,7 +6689,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6707,7 +6718,7 @@
         <v>102</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>104</v>
@@ -6760,7 +6771,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6784,7 +6795,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6795,11 +6806,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6821,10 +6832,10 @@
         <v>101</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>104</v>
@@ -6879,7 +6890,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6914,7 +6925,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6937,19 +6948,19 @@
         <v>56</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -6974,13 +6985,13 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
@@ -6998,7 +7009,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>55</v>
@@ -7016,16 +7027,16 @@
         <v>45</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7033,7 +7044,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7056,19 +7067,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7117,7 +7128,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7135,24 +7146,24 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7175,19 +7186,19 @@
         <v>45</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7212,13 +7223,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7236,7 +7247,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7245,7 +7256,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7260,7 +7271,7 @@
         <v>98</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7271,11 +7282,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7294,19 +7305,19 @@
         <v>45</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7331,13 +7342,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7355,7 +7366,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7373,24 +7384,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7416,16 +7427,16 @@
         <v>45</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7474,7 +7485,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7495,10 +7506,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
Updates across profiles and valuesets
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-PADI-AutopsyObservation.xlsx
+++ b/output/StructureDefinition-PADI-AutopsyObservation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="412">
   <si>
     <t>Path</t>
   </si>
@@ -554,13 +554,7 @@
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>Codes identifying names of simple observations.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
+    <t>http://hl7.org/fhir/us/pacio-adi/ValueSet/PADIAutopsyVS</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -894,6 +888,9 @@
   <si>
     <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   
 If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ bodySite](http://hl7.org/fhir/R4/extension-bodysite.html).</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
   <si>
     <t>Codes describing anatomical locations. May include laterality.</t>
@@ -1268,6 +1265,12 @@
   </si>
   <si>
     <t>*All* code-value and  component.code-component.value pairs need to be taken into account to correctly understand the meaning of the observation.</t>
+  </si>
+  <si>
+    <t>Codes identifying names of simple observations.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
   </si>
   <si>
     <t>&lt; 363787002 |Observable entity| OR @@ -1490,7 +1493,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="60.515625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="50.89453125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="52.7734375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
@@ -2217,7 +2220,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" hidden="true">
+    <row r="7">
       <c r="A7" t="s" s="2">
         <v>83</v>
       </c>
@@ -2227,13 +2230,13 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s" s="2">
         <v>55</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s" s="2">
         <v>45</v>
@@ -3338,13 +3341,11 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="X16" s="2"/>
+      <c r="Y16" t="s" s="2">
         <v>170</v>
-      </c>
-      <c r="X16" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="Y16" t="s" s="2">
-        <v>172</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3377,27 +3378,27 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="AK16" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="AL16" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AM16" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="AL16" t="s" s="2">
+      <c r="AN16" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="AM16" t="s" s="2">
+      <c r="AO16" t="s" s="2">
         <v>176</v>
-      </c>
-      <c r="AN16" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="AO16" t="s" s="2">
-        <v>178</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3420,19 +3421,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="K17" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="L17" t="s" s="2">
         <v>180</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>181</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>182</v>
-      </c>
-      <c r="M17" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>184</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3481,7 +3482,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3496,19 +3497,19 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="AK17" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL17" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="AM17" t="s" s="2">
         <v>185</v>
       </c>
-      <c r="AK17" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL17" t="s" s="2">
+      <c r="AN17" t="s" s="2">
         <v>186</v>
-      </c>
-      <c r="AM17" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="AN17" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3516,7 +3517,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3539,16 +3540,16 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="K18" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="L18" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="M18" t="s" s="2">
         <v>191</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="M18" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3598,7 +3599,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3619,13 +3620,13 @@
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3633,11 +3634,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3656,19 +3657,19 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="K19" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>197</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>199</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
@@ -3717,7 +3718,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3732,19 +3733,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="AK19" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL19" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="AM19" t="s" s="2">
         <v>202</v>
       </c>
-      <c r="AK19" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL19" t="s" s="2">
+      <c r="AN19" t="s" s="2">
         <v>203</v>
-      </c>
-      <c r="AM19" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="AN19" t="s" s="2">
-        <v>205</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3752,11 +3753,11 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3775,19 +3776,19 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="L20" t="s" s="2">
         <v>208</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>209</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="N20" t="s" s="2">
         <v>210</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3836,7 +3837,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3851,19 +3852,19 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AK20" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL20" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="AM20" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="AK20" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL20" t="s" s="2">
+      <c r="AN20" t="s" s="2">
         <v>214</v>
-      </c>
-      <c r="AM20" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="AN20" t="s" s="2">
-        <v>216</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3871,7 +3872,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3894,16 +3895,16 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="K21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>219</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3953,7 +3954,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3974,13 +3975,13 @@
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="AM21" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AN21" t="s" s="2">
         <v>222</v>
-      </c>
-      <c r="AM21" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -3988,7 +3989,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4011,17 +4012,17 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="K22" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="L22" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="K22" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>228</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" t="s" s="2">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4070,7 +4071,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4085,19 +4086,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="AK22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL22" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="AM22" t="s" s="2">
         <v>230</v>
       </c>
-      <c r="AK22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL22" t="s" s="2">
+      <c r="AN22" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="AM22" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4105,7 +4106,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4128,19 +4129,19 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="K23" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>235</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>239</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4189,7 +4190,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4198,7 +4199,7 @@
         <v>55</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>67</v>
@@ -4207,24 +4208,24 @@
         <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AL23" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="AM23" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="AL23" t="s" s="2">
+      <c r="AN23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO23" t="s" s="2">
         <v>242</v>
-      </c>
-      <c r="AM23" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO23" t="s" s="2">
-        <v>244</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4250,16 +4251,16 @@
         <v>154</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="M24" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="N24" t="s" s="2">
         <v>247</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>249</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4284,14 +4285,14 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="X24" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="Y24" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="X24" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="Y24" t="s" s="2">
-        <v>252</v>
-      </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
       </c>
@@ -4308,7 +4309,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4317,7 +4318,7 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
@@ -4332,7 +4333,7 @@
         <v>98</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
@@ -4343,11 +4344,11 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4369,16 +4370,16 @@
         <v>154</v>
       </c>
       <c r="K25" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="L25" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="M25" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="L25" t="s" s="2">
+      <c r="N25" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4403,13 +4404,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4427,7 +4428,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4445,24 +4446,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="AL25" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AM25" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="AL25" t="s" s="2">
+      <c r="AN25" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO25" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="AM25" t="s" s="2">
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="AN25" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO25" t="s" s="2">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="26" hidden="true">
-      <c r="A26" t="s" s="2">
-        <v>267</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4476,7 +4477,7 @@
         <v>44</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>45</v>
@@ -4485,19 +4486,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="K26" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>270</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>272</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4546,7 +4547,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4567,10 +4568,10 @@
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -4581,7 +4582,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4607,13 +4608,13 @@
         <v>154</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="L27" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="M27" t="s" s="2">
         <v>276</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>278</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4639,14 +4640,14 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>170</v>
+        <v>277</v>
       </c>
       <c r="X27" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="Y27" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="Y27" t="s" s="2">
-        <v>280</v>
-      </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4663,7 +4664,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4681,24 +4682,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="AL27" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="AL27" t="s" s="2">
+      <c r="AM27" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="AM27" t="s" s="2">
+      <c r="AN27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO27" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="AN27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO27" t="s" s="2">
-        <v>284</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4724,16 +4725,16 @@
         <v>154</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>287</v>
       </c>
-      <c r="M28" t="s" s="2">
+      <c r="N28" t="s" s="2">
         <v>288</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>289</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4758,14 +4759,14 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>170</v>
+        <v>277</v>
       </c>
       <c r="X28" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="Y28" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="Y28" t="s" s="2">
-        <v>291</v>
-      </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
       </c>
@@ -4782,7 +4783,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4803,10 +4804,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AM28" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="AM28" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4817,7 +4818,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4840,16 +4841,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="K29" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>296</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>297</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>298</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4899,7 +4900,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4917,24 +4918,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AL29" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="AL29" t="s" s="2">
+      <c r="AM29" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="AM29" t="s" s="2">
+      <c r="AN29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO29" t="s" s="2">
         <v>301</v>
-      </c>
-      <c r="AN29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO29" t="s" s="2">
-        <v>302</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4957,16 +4958,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5016,7 +5017,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5034,24 +5035,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="AL30" t="s" s="2">
         <v>308</v>
       </c>
-      <c r="AL30" t="s" s="2">
+      <c r="AM30" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="AM30" t="s" s="2">
+      <c r="AN30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO30" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>311</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5074,19 +5075,19 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>317</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5135,7 +5136,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5147,19 +5148,19 @@
         <v>45</v>
       </c>
       <c r="AI31" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL31" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="AJ31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL31" t="s" s="2">
+      <c r="AM31" t="s" s="2">
         <v>319</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>320</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5170,7 +5171,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5196,10 +5197,10 @@
         <v>57</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5250,7 +5251,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5274,7 +5275,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5285,7 +5286,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5314,7 +5315,7 @@
         <v>102</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>104</v>
@@ -5367,7 +5368,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5391,7 +5392,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5402,11 +5403,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5428,10 +5429,10 @@
         <v>101</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>331</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>332</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>104</v>
@@ -5486,7 +5487,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5521,7 +5522,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5544,13 +5545,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="K35" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="K35" t="s" s="2">
+      <c r="L35" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>337</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5601,7 +5602,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5610,7 +5611,7 @@
         <v>55</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>67</v>
@@ -5622,10 +5623,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>339</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>340</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5636,7 +5637,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5659,13 +5660,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>342</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>343</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5716,7 +5717,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5725,7 +5726,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5737,10 +5738,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5751,7 +5752,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5777,16 +5778,16 @@
         <v>154</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>346</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>347</v>
       </c>
-      <c r="M37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>348</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>349</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5814,11 +5815,11 @@
         <v>79</v>
       </c>
       <c r="X37" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="Y37" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="Y37" t="s" s="2">
-        <v>351</v>
-      </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5835,7 +5836,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5853,13 +5854,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="AL37" t="s" s="2">
-        <v>353</v>
-      </c>
       <c r="AM37" t="s" s="2">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5870,7 +5871,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5896,16 +5897,16 @@
         <v>154</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>356</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>357</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>358</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5930,14 +5931,14 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>170</v>
+        <v>277</v>
       </c>
       <c r="X38" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="Y38" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="Y38" t="s" s="2">
-        <v>360</v>
-      </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
       </c>
@@ -5954,7 +5955,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5972,13 +5973,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="AL38" t="s" s="2">
-        <v>353</v>
-      </c>
       <c r="AM38" t="s" s="2">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5989,7 +5990,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6012,17 +6013,17 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>362</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>363</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>364</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6071,7 +6072,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6095,7 +6096,7 @@
         <v>45</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6106,7 +6107,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6132,10 +6133,10 @@
         <v>57</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>368</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>369</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -6186,7 +6187,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6207,10 +6208,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6221,7 +6222,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6244,16 +6245,16 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="K41" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="L41" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>375</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -6303,7 +6304,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6324,10 +6325,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="AM41" t="s" s="2">
         <v>376</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>377</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6338,7 +6339,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6361,16 +6362,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>379</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6420,7 +6421,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6441,10 +6442,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6455,7 +6456,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6478,19 +6479,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>385</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>386</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>387</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>388</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -6539,7 +6540,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6560,10 +6561,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="AM43" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="AM43" t="s" s="2">
-        <v>390</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6574,7 +6575,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6600,10 +6601,10 @@
         <v>57</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6654,7 +6655,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6678,7 +6679,7 @@
         <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6689,7 +6690,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6718,7 +6719,7 @@
         <v>102</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>104</v>
@@ -6771,7 +6772,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6795,7 +6796,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6806,11 +6807,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6832,10 +6833,10 @@
         <v>101</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>331</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>332</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>104</v>
@@ -6890,7 +6891,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6925,7 +6926,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6951,13 +6952,13 @@
         <v>154</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>396</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>397</v>
       </c>
       <c r="N47" t="s" s="2">
         <v>168</v>
@@ -6985,13 +6986,13 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>170</v>
+        <v>277</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>171</v>
+        <v>397</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>172</v>
+        <v>398</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
@@ -7009,7 +7010,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>55</v>
@@ -7027,16 +7028,16 @@
         <v>45</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AL47" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="AM47" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="AN47" t="s" s="2">
         <v>175</v>
-      </c>
-      <c r="AM47" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="AN47" t="s" s="2">
-        <v>177</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7044,7 +7045,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7067,19 +7068,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="K48" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>235</v>
       </c>
-      <c r="K48" t="s" s="2">
-        <v>400</v>
-      </c>
-      <c r="L48" t="s" s="2">
+      <c r="M48" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="N48" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>401</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>239</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7128,7 +7129,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7146,24 +7147,24 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AL48" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>242</v>
-      </c>
-      <c r="AM48" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>244</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7189,16 +7190,16 @@
         <v>154</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7223,14 +7224,14 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="X49" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="Y49" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="X49" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="Y49" t="s" s="2">
-        <v>252</v>
-      </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7247,7 +7248,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7256,7 +7257,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7271,7 +7272,7 @@
         <v>98</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7282,11 +7283,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7308,16 +7309,16 @@
         <v>154</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="N50" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7342,13 +7343,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7366,7 +7367,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7384,24 +7385,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AM50" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="AL50" t="s" s="2">
+      <c r="AN50" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO50" t="s" s="2">
         <v>264</v>
-      </c>
-      <c r="AM50" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO50" t="s" s="2">
-        <v>266</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7427,16 +7428,16 @@
         <v>45</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M51" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="N51" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>317</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7485,7 +7486,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7506,10 +7507,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="AM51" t="s" s="2">
         <v>319</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>320</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>

</xml_diff>